<commit_message>
updated human study results
</commit_message>
<xml_diff>
--- a/notebooks/human_study.xlsx
+++ b/notebooks/human_study.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="93">
   <si>
     <t>Timestamp</t>
   </si>
@@ -236,6 +236,60 @@
   </si>
   <si>
     <t>a b</t>
+  </si>
+  <si>
+    <t>bbaabbabb</t>
+  </si>
+  <si>
+    <t>[]())(</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>b a</t>
+  </si>
+  <si>
+    <t>][()</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>][[]</t>
+  </si>
+  <si>
+    <t>()</t>
+  </si>
+  <si>
+    <t>aaba, aaab</t>
+  </si>
+  <si>
+    <t>bbbbaa, bbbbbbbbaaaa</t>
+  </si>
+  <si>
+    <t>baabbaab, baabbaabbaab, baabbaabbaabbaab</t>
+  </si>
+  <si>
+    <t>)[](</t>
+  </si>
+  <si>
+    <t>(([])), [[]]</t>
+  </si>
+  <si>
+    <t>)(][)(, [()()]</t>
+  </si>
+  <si>
+    <t>)()()(</t>
+  </si>
+  <si>
+    <t>abba, ababbaa</t>
+  </si>
+  <si>
+    <t>baab, abbaab</t>
+  </si>
+  <si>
+    <t>babaab</t>
   </si>
 </sst>
 </file>
@@ -1049,6 +1103,170 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>45430.484464548616</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>45433.56760267361</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>45433.58018291667</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>45433.688659340274</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>